<commit_message>
Initial CRUD work on Horses
</commit_message>
<xml_diff>
--- a/SchemaDef.xlsx
+++ b/SchemaDef.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vtchief/Development/CCRHorses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F04276-18A2-6A47-B774-038CBE2336C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8582EFB9-2027-DB4A-813F-F0991C22FF3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7280" yWindow="1300" windowWidth="27640" windowHeight="19220" xr2:uid="{EF7D8736-F762-2646-80E2-687D23334C5B}"/>
+    <workbookView xWindow="37720" yWindow="1660" windowWidth="27640" windowHeight="19220" xr2:uid="{EF7D8736-F762-2646-80E2-687D23334C5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
   <si>
     <t>CCR Horse Inventory</t>
   </si>
@@ -181,6 +181,30 @@
   </si>
   <si>
     <t>RegisteredName</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>ActiveComments</t>
+  </si>
+  <si>
+    <t>Markings</t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t>BestFriend</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Height</t>
   </si>
 </sst>
 </file>
@@ -204,12 +228,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -224,9 +254,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D0146F6-B1AD-9941-A8B9-85590206D2F1}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A4" sqref="A4:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -554,125 +585,141 @@
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>42</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B17" t="s">
         <v>5</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C17" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D17" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -680,57 +727,54 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" t="s">
-        <v>16</v>
+      <c r="D21" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>17</v>
+      <c r="D22" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>23</v>
+      <c r="D23" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
-        <v>7</v>
+      <c r="D24" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>14</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -739,107 +783,154 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C28" t="s">
-        <v>45</v>
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C30" t="s">
-        <v>7</v>
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>22</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B39" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C33" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C34" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C35" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C36" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>22</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B44" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C38" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C39" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C40" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C41" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>22</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B49" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C43" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C44" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C51" t="s">
         <v>36</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D51" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C45" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>